<commit_message>
change job list -week9
</commit_message>
<xml_diff>
--- a/Job List.xlsx
+++ b/Job List.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Week 2" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="weeek3" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="week8" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="week9" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t xml:space="preserve">problems</t>
   </si>
@@ -96,25 +97,34 @@
     <t xml:space="preserve">tasks</t>
   </si>
   <si>
+    <t xml:space="preserve">objectives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study ARCore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARCore functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">android basic knowledge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study OpenCV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design GUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design init GUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implement GUI</t>
+  </si>
+  <si>
     <t xml:space="preserve">estimated hours</t>
   </si>
   <si>
     <t xml:space="preserve">remaining effort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">study ARCore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">study OpenCV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">design GUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">design init GUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implement GUI</t>
   </si>
 </sst>
 </file>
@@ -169,11 +179,81 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -203,7 +283,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -216,7 +296,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,11 +308,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -322,7 +450,7 @@
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="43.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -406,7 +534,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="45.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,28 +601,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.66"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="C1" s="3"/>
       <c r="D1" s="4" t="n">
         <f aca="false">DATE(2018,10,26)</f>
@@ -511,60 +642,68 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="C2" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6"/>
+      <c r="B3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="C3" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="E4" s="0" t="n">
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="F4" s="12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
         <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
@@ -579,27 +718,274 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="0" t="s">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13"/>
+      <c r="B6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">SUM(C2:C6)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">SUM(C2:C6)</f>
+        <v>33</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">SUM(D2:D6)</f>
+        <v>31</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">SUM(E2:E6)</f>
         <v>30</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F8" s="0" t="n">
+        <f aca="false">SUM(F2:F6)</f>
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.66"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="4" t="n">
+        <f aca="false">DATE(2018,10,29)</f>
+        <v>43402</v>
+      </c>
+      <c r="E1" s="4" t="n">
+        <f aca="false">D1+1</f>
+        <v>43403</v>
+      </c>
+      <c r="F1" s="4" t="n">
+        <f aca="false">E1+1</f>
+        <v>43404</v>
+      </c>
+      <c r="G1" s="4" t="n">
+        <f aca="false">F1+1</f>
+        <v>43405</v>
+      </c>
+      <c r="H1" s="4" t="n">
+        <f aca="false">G1+1</f>
+        <v>43406</v>
+      </c>
+      <c r="I1" s="4" t="n">
+        <f aca="false">H1+1</f>
+        <v>43407</v>
+      </c>
+      <c r="J1" s="4" t="n">
+        <f aca="false">I1+1</f>
+        <v>43408</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6"/>
+      <c r="B3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" s="12" t="n">
+        <v>8</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13"/>
+      <c r="B6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G6" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="19" t="n">
+        <f aca="false">SUM(C2:C6)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="19" t="n">
+        <f aca="false">SUM(C2:C6)</f>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="A5:A6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>